<commit_message>
Changes during  Sam meeting..
</commit_message>
<xml_diff>
--- a/src/technology/ldes/ldes.xlsx
+++ b/src/technology/ldes/ldes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tghosh/Library/CloudStorage/OneDrive-NREL/work_NREL/tyche/src/technology/ldes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB41EE8-06CD-534F-90CD-C124ADB0363A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1337E9D-A728-1B4E-84F5-7E2A86C1F47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="760" windowWidth="31960" windowHeight="19860" activeTab="4" xr2:uid="{021BDB00-52DC-4A4E-ACEA-9258FAE2C700}"/>
+    <workbookView xWindow="-45780" yWindow="-5280" windowWidth="37940" windowHeight="24820" activeTab="4" xr2:uid="{021BDB00-52DC-4A4E-ACEA-9258FAE2C700}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="105">
   <si>
     <t>Technology</t>
   </si>
@@ -206,9 +206,6 @@
     <t>High R&amp;D Electrolysis</t>
   </si>
   <si>
-    <t>CF rectifier</t>
-  </si>
-  <si>
     <t>CF Electrolysis</t>
   </si>
   <si>
@@ -321,6 +318,45 @@
   </si>
   <si>
     <t>Fixed cost BoS 3</t>
+  </si>
+  <si>
+    <t>Efficiency of rectifier = 0.95</t>
+  </si>
+  <si>
+    <t>Efficiency of electrolysis = 0.40</t>
+  </si>
+  <si>
+    <t>CF of rectifier does not exists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balance of systems can be a warehouse with stacked electrolyzers feeding into hydrogen into the output into the cavern. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOS will not have an input and output. </t>
+  </si>
+  <si>
+    <t>Efficiency and CF does not exist</t>
+  </si>
+  <si>
+    <t>Fixed and Variable cost to an O&amp;M</t>
+  </si>
+  <si>
+    <t>Change of scales when something happens in downstream</t>
+  </si>
+  <si>
+    <t>input(0)</t>
+  </si>
+  <si>
+    <t>output(0)</t>
+  </si>
+  <si>
+    <t>Efficiency rectifier</t>
+  </si>
+  <si>
+    <t>parameter[0]</t>
+  </si>
+  <si>
+    <t>[0.95,0.96,0.98]</t>
   </si>
 </sst>
 </file>
@@ -695,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF408755-AA2A-5A47-B57D-CAC214069608}">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView zoomScale="232" zoomScaleNormal="232" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -746,7 +782,10 @@
         <v>51</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -765,6 +804,9 @@
       <c r="E3">
         <v>1</v>
       </c>
+      <c r="G3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -782,6 +824,9 @@
       <c r="E4">
         <v>1</v>
       </c>
+      <c r="G4" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -794,7 +839,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -862,7 +907,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -879,7 +924,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -913,7 +958,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -930,7 +975,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -992,13 +1037,13 @@
         <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>69</v>
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1012,7 +1057,7 @@
         <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
         <v>51</v>
@@ -1029,7 +1074,7 @@
         <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
         <v>51</v>
@@ -1046,10 +1091,10 @@
         <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s">
-        <v>51</v>
+        <v>11</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1063,10 +1108,10 @@
         <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>74</v>
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1080,7 +1125,7 @@
         <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
         <v>51</v>
@@ -1097,10 +1142,10 @@
         <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" t="s">
-        <v>51</v>
+        <v>10</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1116,8 +1161,8 @@
       <c r="C24" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>48</v>
+      <c r="D24" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1134,7 +1179,7 @@
         <v>10</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1151,7 +1196,7 @@
         <v>10</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1168,7 +1213,7 @@
         <v>10</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1202,7 +1247,7 @@
         <v>10</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -1219,7 +1264,7 @@
         <v>10</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1236,7 +1281,7 @@
         <v>10</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1247,13 +1292,13 @@
         <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>68</v>
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>51</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1264,13 +1309,13 @@
         <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>69</v>
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>51</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1284,7 +1329,7 @@
         <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D34" t="s">
         <v>51</v>
@@ -1301,10 +1346,10 @@
         <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" t="s">
-        <v>51</v>
+        <v>11</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1318,7 +1363,7 @@
         <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D36" t="s">
         <v>51</v>
@@ -1335,10 +1380,10 @@
         <v>53</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>74</v>
+        <v>13</v>
+      </c>
+      <c r="D37" t="s">
+        <v>51</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -1352,10 +1397,10 @@
         <v>53</v>
       </c>
       <c r="C38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" t="s">
-        <v>51</v>
+        <v>10</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -1369,10 +1414,10 @@
         <v>53</v>
       </c>
       <c r="C39" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" t="s">
-        <v>51</v>
+        <v>10</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -1388,8 +1433,8 @@
       <c r="C40" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>48</v>
+      <c r="D40" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -1406,7 +1451,7 @@
         <v>10</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -1423,7 +1468,7 @@
         <v>10</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -1440,7 +1485,7 @@
         <v>10</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -1457,7 +1502,7 @@
         <v>10</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -1474,7 +1519,7 @@
         <v>10</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -1491,60 +1536,9 @@
         <v>10</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47" t="s">
-        <v>53</v>
-      </c>
-      <c r="C47" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>53</v>
-      </c>
-      <c r="C48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>47</v>
-      </c>
-      <c r="B49" t="s">
-        <v>53</v>
-      </c>
-      <c r="C49" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E49">
         <v>1</v>
       </c>
     </row>
@@ -1558,7 +1552,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView zoomScale="204" zoomScaleNormal="204" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1637,7 +1631,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -1651,7 +1645,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1679,7 +1673,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1693,7 +1687,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -1707,7 +1701,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -1721,7 +1715,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11">
         <v>9</v>
@@ -1752,7 +1746,7 @@
         <v>51</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1859,7 +1853,7 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -1913,10 +1907,10 @@
         <v>41</v>
       </c>
       <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
         <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1924,10 +1918,10 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1937,10 +1931,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D60756-8727-469C-BF07-9640ADCA9D3D}">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="187" zoomScaleNormal="187" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1951,7 +1945,7 @@
     <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1974,7 +1968,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1982,19 +1976,19 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -2002,7 +1996,7 @@
         <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2010,8 +2004,11 @@
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -2019,7 +2016,7 @@
         <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -2027,8 +2024,11 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -2044,8 +2044,11 @@
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -2061,8 +2064,11 @@
       <c r="E6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -2070,7 +2076,7 @@
         <v>39</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -2078,8 +2084,11 @@
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -2087,7 +2096,7 @@
         <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -2095,8 +2104,11 @@
       <c r="E8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -2104,7 +2116,7 @@
         <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -2113,7 +2125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -2121,7 +2133,7 @@
         <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -2130,7 +2142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -2138,7 +2150,7 @@
         <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11">
         <v>9</v>
@@ -2146,8 +2158,11 @@
       <c r="E11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -2155,7 +2170,7 @@
         <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -2164,7 +2179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -2172,7 +2187,7 @@
         <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13">
         <v>11</v>
@@ -2181,7 +2196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -2189,7 +2204,7 @@
         <v>39</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14">
         <v>12</v>
@@ -2198,7 +2213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -2206,7 +2221,7 @@
         <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15">
         <v>13</v>
@@ -2215,7 +2230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -2223,7 +2238,7 @@
         <v>39</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D16">
         <v>14</v>
@@ -2231,6 +2246,12 @@
       <c r="E16">
         <v>1</v>
       </c>
+      <c r="G16" t="s">
+        <v>103</v>
+      </c>
+      <c r="I16" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -2240,7 +2261,7 @@
         <v>39</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D17">
         <v>15</v>
@@ -2257,7 +2278,7 @@
         <v>39</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D18">
         <v>16</v>
@@ -2274,7 +2295,7 @@
         <v>39</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D19">
         <v>17</v>
@@ -2291,7 +2312,7 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D20">
         <v>18</v>
@@ -2308,7 +2329,7 @@
         <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D21">
         <v>19</v>
@@ -2325,7 +2346,7 @@
         <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D22">
         <v>20</v>
@@ -2342,7 +2363,7 @@
         <v>39</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23">
         <v>21</v>
@@ -2359,7 +2380,7 @@
         <v>39</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D24">
         <v>22</v>
@@ -2376,7 +2397,7 @@
         <v>39</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D25">
         <v>23</v>
@@ -2393,7 +2414,7 @@
         <v>39</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D26">
         <v>24</v>
@@ -2410,7 +2431,7 @@
         <v>39</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D27">
         <v>25</v>
@@ -2427,7 +2448,7 @@
         <v>39</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D28">
         <v>26</v>
@@ -2444,13 +2465,13 @@
         <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -2461,7 +2482,7 @@
         <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -2478,7 +2499,7 @@
         <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -2495,7 +2516,7 @@
         <v>52</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D32">
         <v>3</v>
@@ -2512,7 +2533,7 @@
         <v>52</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D33">
         <v>4</v>
@@ -2529,7 +2550,7 @@
         <v>52</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D34">
         <v>5</v>
@@ -2546,7 +2567,7 @@
         <v>52</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D35">
         <v>6</v>
@@ -2563,7 +2584,7 @@
         <v>52</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D36">
         <v>7</v>
@@ -2580,7 +2601,7 @@
         <v>52</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D37">
         <v>8</v>
@@ -2597,7 +2618,7 @@
         <v>52</v>
       </c>
       <c r="C38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D38">
         <v>9</v>
@@ -2614,7 +2635,7 @@
         <v>52</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D39">
         <v>10</v>
@@ -2631,7 +2652,7 @@
         <v>52</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D40">
         <v>11</v>
@@ -2648,7 +2669,7 @@
         <v>52</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D41">
         <v>12</v>
@@ -2665,7 +2686,7 @@
         <v>52</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D42">
         <v>13</v>
@@ -2682,7 +2703,7 @@
         <v>52</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D43">
         <v>14</v>
@@ -2699,7 +2720,7 @@
         <v>52</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D44">
         <v>15</v>
@@ -2716,7 +2737,7 @@
         <v>52</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D45">
         <v>16</v>
@@ -2733,7 +2754,7 @@
         <v>52</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D46">
         <v>17</v>
@@ -2750,7 +2771,7 @@
         <v>52</v>
       </c>
       <c r="C47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D47">
         <v>18</v>
@@ -2767,7 +2788,7 @@
         <v>52</v>
       </c>
       <c r="C48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D48">
         <v>19</v>
@@ -2784,7 +2805,7 @@
         <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D49">
         <v>20</v>
@@ -2801,7 +2822,7 @@
         <v>52</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D50">
         <v>21</v>
@@ -2818,7 +2839,7 @@
         <v>52</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D51">
         <v>22</v>
@@ -2835,7 +2856,7 @@
         <v>52</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D52">
         <v>23</v>
@@ -2852,7 +2873,7 @@
         <v>52</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D53">
         <v>24</v>
@@ -2869,7 +2890,7 @@
         <v>52</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D54">
         <v>25</v>
@@ -2886,7 +2907,7 @@
         <v>52</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D55">
         <v>26</v>
@@ -2903,13 +2924,13 @@
         <v>53</v>
       </c>
       <c r="C56" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="D56">
         <v>0</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -2920,7 +2941,7 @@
         <v>53</v>
       </c>
       <c r="C57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -2937,7 +2958,7 @@
         <v>53</v>
       </c>
       <c r="C58" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D58">
         <v>2</v>
@@ -2954,7 +2975,7 @@
         <v>53</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D59">
         <v>3</v>
@@ -2971,7 +2992,7 @@
         <v>53</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D60">
         <v>4</v>
@@ -2988,7 +3009,7 @@
         <v>53</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D61">
         <v>5</v>
@@ -3005,7 +3026,7 @@
         <v>53</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D62">
         <v>6</v>
@@ -3022,7 +3043,7 @@
         <v>53</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D63">
         <v>7</v>
@@ -3039,7 +3060,7 @@
         <v>53</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D64">
         <v>8</v>
@@ -3056,7 +3077,7 @@
         <v>53</v>
       </c>
       <c r="C65" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D65">
         <v>9</v>
@@ -3073,7 +3094,7 @@
         <v>53</v>
       </c>
       <c r="C66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D66">
         <v>10</v>
@@ -3090,7 +3111,7 @@
         <v>53</v>
       </c>
       <c r="C67" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D67">
         <v>11</v>
@@ -3107,7 +3128,7 @@
         <v>53</v>
       </c>
       <c r="C68" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D68">
         <v>12</v>
@@ -3124,7 +3145,7 @@
         <v>53</v>
       </c>
       <c r="C69" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D69">
         <v>13</v>
@@ -3141,7 +3162,7 @@
         <v>53</v>
       </c>
       <c r="C70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D70">
         <v>14</v>
@@ -3158,7 +3179,7 @@
         <v>53</v>
       </c>
       <c r="C71" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D71">
         <v>15</v>
@@ -3175,7 +3196,7 @@
         <v>53</v>
       </c>
       <c r="C72" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D72">
         <v>16</v>
@@ -3192,7 +3213,7 @@
         <v>53</v>
       </c>
       <c r="C73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D73">
         <v>17</v>
@@ -3209,7 +3230,7 @@
         <v>53</v>
       </c>
       <c r="C74" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D74">
         <v>18</v>
@@ -3226,7 +3247,7 @@
         <v>53</v>
       </c>
       <c r="C75" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D75">
         <v>19</v>
@@ -3243,7 +3264,7 @@
         <v>53</v>
       </c>
       <c r="C76" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D76">
         <v>20</v>
@@ -3260,7 +3281,7 @@
         <v>53</v>
       </c>
       <c r="C77" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D77">
         <v>21</v>
@@ -3277,7 +3298,7 @@
         <v>53</v>
       </c>
       <c r="C78" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D78">
         <v>22</v>
@@ -3294,7 +3315,7 @@
         <v>53</v>
       </c>
       <c r="C79" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D79">
         <v>23</v>
@@ -3311,7 +3332,7 @@
         <v>53</v>
       </c>
       <c r="C80" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D80">
         <v>24</v>
@@ -3328,7 +3349,7 @@
         <v>53</v>
       </c>
       <c r="C81" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D81">
         <v>25</v>
@@ -3345,7 +3366,7 @@
         <v>53</v>
       </c>
       <c r="C82" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D82">
         <v>26</v>
@@ -3494,10 +3515,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" t="s">
-        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -3508,10 +3529,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
         <v>40</v>

</xml_diff>